<commit_message>
Changement dans le tableau de synthèse
</commit_message>
<xml_diff>
--- a/Tableau-de-synthèse/8 - BTS SIO - Annexe 8-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2024.xlsx
+++ b/Tableau-de-synthèse/8 - BTS SIO - Annexe 8-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minei\Documents\portfolio_cybersecurite_elegant\Tableau de synthèse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minei\Documents\portfolio_cybersecurite_elegant\Tableau-de-synthèse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C584E03-8A2E-4EA5-B5CA-ECC3DDD365A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E99703-9532-4643-B98E-C476BD297780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
     <t>Centre de formation : Le Rebours</t>
@@ -141,9 +138,6 @@
     <t>Lien Portfolio : https://florentmineiro.github.io/portfolio/</t>
   </si>
   <si>
-    <t>Projet application IMMOSYNC</t>
-  </si>
-  <si>
     <t>19/05/2025 au 27/06/2025</t>
   </si>
   <si>
@@ -162,9 +156,6 @@
     <t>Création site vitrine pour marque vitrine</t>
   </si>
   <si>
-    <t>coming soon</t>
-  </si>
-  <si>
     <t>Septembre 2024 à Novembre 2024</t>
   </si>
   <si>
@@ -174,16 +165,13 @@
     <t xml:space="preserve">Stage de fin d'année :refonte de site sur wix </t>
   </si>
   <si>
-    <t>Stage de 2ème année : refonte de site sur Worpress</t>
-  </si>
-  <si>
-    <t>05/01/2026 au 20/02/2026</t>
-  </si>
-  <si>
     <t>Réalisation de Portfolio</t>
   </si>
   <si>
     <t>02/09/2025 à aujourd'hui</t>
+  </si>
+  <si>
+    <t>N° candidat : 02541488301</t>
   </si>
 </sst>
 </file>
@@ -971,25 +959,25 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>145398</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>120068</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>439284</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>189090</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>799518</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>410948</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>757524</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>412290</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="5" name="Encre 4">
+            <xdr14:cNvPr id="11" name="Encre 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E07F51B5-5DB3-2AF1-52AC-34FC299187CA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D3B7F00-67F7-26E0-82CE-7C881F80383B}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -997,18 +985,18 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="11498760" y="10225327"/>
-            <a:ext cx="654120" cy="290880"/>
+            <a:off x="10487880" y="9112511"/>
+            <a:ext cx="318240" cy="223200"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
       <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="5" name="Encre 4">
+            <xdr:cNvPr id="11" name="Encre 10">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E07F51B5-5DB3-2AF1-52AC-34FC299187CA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D3B7F00-67F7-26E0-82CE-7C881F80383B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1022,8 +1010,8 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11462760" y="10189327"/>
-              <a:ext cx="725760" cy="362520"/>
+              <a:off x="10479230" y="9103871"/>
+              <a:ext cx="335900" cy="240840"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1037,24 +1025,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>186078</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>207548</xdr:rowOff>
+      <xdr:colOff>512142</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>167130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1029558</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>459908</xdr:rowOff>
+      <xdr:colOff>824622</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>438210</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="9" name="Encre 8">
+            <xdr14:cNvPr id="15" name="Encre 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EAB53CE-8744-94E7-83E4-8DCF030CC64E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C83C9F4-B448-B837-20A5-6D770290F0EE}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1062,18 +1050,18 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="11539440" y="10312807"/>
-            <a:ext cx="843480" cy="252360"/>
+            <a:off x="11864160" y="9090551"/>
+            <a:ext cx="312480" cy="271080"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
       <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="9" name="Encre 8">
+            <xdr:cNvPr id="15" name="Encre 14">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EAB53CE-8744-94E7-83E4-8DCF030CC64E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C83C9F4-B448-B837-20A5-6D770290F0EE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1087,8 +1075,8 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11503440" y="10276807"/>
-              <a:ext cx="915120" cy="324000"/>
+              <a:off x="11855520" y="9081551"/>
+              <a:ext cx="330120" cy="288720"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1102,24 +1090,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>361071</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>163715</xdr:rowOff>
+      <xdr:colOff>294620</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>111330</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>963711</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>486635</xdr:rowOff>
+      <xdr:colOff>690980</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>303570</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="13" name="Encre 12">
+            <xdr14:cNvPr id="16" name="Encre 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B2D23AC-DA38-0D27-5166-DFCA8A1790F2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFDE4112-28E5-D96D-9EB8-884766AB2F8D}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1127,18 +1115,18 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="14320123" y="10268974"/>
-            <a:ext cx="602640" cy="322920"/>
+            <a:off x="14253480" y="9034751"/>
+            <a:ext cx="396360" cy="192240"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
       <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="13" name="Encre 12">
+            <xdr:cNvPr id="16" name="Encre 15">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B2D23AC-DA38-0D27-5166-DFCA8A1790F2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFDE4112-28E5-D96D-9EB8-884766AB2F8D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1152,8 +1140,203 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="14284462" y="10233334"/>
-              <a:ext cx="674323" cy="394560"/>
+              <a:off x="14244840" y="9026111"/>
+              <a:ext cx="414000" cy="209880"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>378860</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>155610</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>635540</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>352890</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="19" name="Encre 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E065EA6-F1A8-443B-237B-60A339EA97DD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14337720" y="9079031"/>
+            <a:ext cx="256680" cy="197280"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="19" name="Encre 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E065EA6-F1A8-443B-237B-60A339EA97DD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14328720" y="9070391"/>
+              <a:ext cx="274320" cy="214920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>512142</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>178114</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>836142</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>448834</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="23" name="Encre 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{285A9A91-08A4-C21A-646B-290C5A44204C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11864160" y="9613991"/>
+            <a:ext cx="324000" cy="270720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="23" name="Encre 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{285A9A91-08A4-C21A-646B-290C5A44204C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11855510" y="9605362"/>
+              <a:ext cx="341660" cy="288337"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>608900</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>233554</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>891140</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>433714</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="26" name="Encre 25">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63923DC0-0FE5-2FC9-C17B-3C9C1207DD40}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14567760" y="9669431"/>
+            <a:ext cx="282240" cy="200160"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="26" name="Encre 25">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63923DC0-0FE5-2FC9-C17B-3C9C1207DD40}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14559120" y="9660791"/>
+              <a:ext cx="299880" cy="217800"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1167,24 +1350,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>275732</xdr:colOff>
+      <xdr:colOff>559966</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>98047</xdr:rowOff>
+      <xdr:rowOff>122498</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>996452</xdr:colOff>
+      <xdr:colOff>925366</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>345367</xdr:rowOff>
+      <xdr:rowOff>336698</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="21" name="Encre 20">
+            <xdr14:cNvPr id="30" name="Encre 29">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEE26F00-07ED-4D02-8136-C79027F3F8C8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AC97A81-4F83-241B-44C8-B9470FC008A5}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1192,33 +1375,163 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="7720560" y="10706926"/>
-            <a:ext cx="720720" cy="247320"/>
+            <a:off x="8001720" y="10070831"/>
+            <a:ext cx="365400" cy="214200"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
       <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="21" name="Encre 20">
+            <xdr:cNvPr id="30" name="Encre 29">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEE26F00-07ED-4D02-8136-C79027F3F8C8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AC97A81-4F83-241B-44C8-B9470FC008A5}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7684560" y="10671286"/>
-              <a:ext cx="792360" cy="318960"/>
+              <a:off x="7992720" y="10061831"/>
+              <a:ext cx="383040" cy="231840"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>490182</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>808062</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>416618</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="34" name="Encre 33">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92128C78-56E0-9C55-175D-27D6D2244611}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11842200" y="10126271"/>
+            <a:ext cx="317880" cy="238680"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="34" name="Encre 33">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92128C78-56E0-9C55-175D-27D6D2244611}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11833200" y="10117271"/>
+              <a:ext cx="335520" cy="256320"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>534462</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>211418</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>813102</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>389978</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="36" name="Encre 35">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0C1D01-4E31-013B-E14C-43EA25BEA4B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11886480" y="10159751"/>
+            <a:ext cx="278640" cy="178560"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="36" name="Encre 35">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0C1D01-4E31-013B-E14C-43EA25BEA4B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11877480" y="10150751"/>
+              <a:ext cx="296280" cy="196200"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1232,24 +1545,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>361028</xdr:colOff>
+      <xdr:colOff>449420</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>196968</xdr:rowOff>
+      <xdr:rowOff>177938</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1139348</xdr:colOff>
+      <xdr:colOff>913820</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>490008</xdr:rowOff>
+      <xdr:rowOff>415898</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="27" name="Encre 26">
+            <xdr14:cNvPr id="39" name="Encre 38">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2E1E017-EF94-CCB5-2444-15C24671674D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E442F60A-3993-D9C5-6296-CA4B8B6F160B}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1257,33 +1570,33 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="14320080" y="10805847"/>
-            <a:ext cx="778320" cy="293040"/>
+            <a:off x="14408280" y="10126271"/>
+            <a:ext cx="464400" cy="237960"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
       <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="27" name="Encre 26">
+            <xdr:cNvPr id="39" name="Encre 38">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2E1E017-EF94-CCB5-2444-15C24671674D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E442F60A-3993-D9C5-6296-CA4B8B6F160B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="14284063" y="10769891"/>
-              <a:ext cx="849993" cy="364592"/>
+              <a:off x="14399640" y="10117271"/>
+              <a:ext cx="482040" cy="255600"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1297,24 +1610,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>253772</xdr:colOff>
+      <xdr:colOff>437566</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>109482</xdr:rowOff>
+      <xdr:rowOff>244722</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>843092</xdr:colOff>
+      <xdr:colOff>925366</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>448962</xdr:rowOff>
+      <xdr:rowOff>405642</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="41" name="Encre 40">
+            <xdr14:cNvPr id="42" name="Encre 41">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93D66B79-0BE6-6CDD-AF62-8BCF19873356}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23DE672A-ECE1-1809-99A2-A56DA6753205}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1322,33 +1635,98 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="7698600" y="11221982"/>
-            <a:ext cx="589320" cy="339480"/>
+            <a:off x="7879320" y="10705511"/>
+            <a:ext cx="487800" cy="160920"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
       <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="41" name="Encre 40">
+            <xdr:cNvPr id="42" name="Encre 41">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93D66B79-0BE6-6CDD-AF62-8BCF19873356}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23DE672A-ECE1-1809-99A2-A56DA6753205}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7662960" y="11185982"/>
-              <a:ext cx="660960" cy="411120"/>
+              <a:off x="7870320" y="10696511"/>
+              <a:ext cx="505440" cy="178560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>534406</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>111162</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>858046</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>434802</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="45" name="Encre 44">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81253D77-1075-BCD8-C25B-DE1AED8A63D3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7976160" y="10571951"/>
+            <a:ext cx="323640" cy="323640"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="45" name="Encre 44">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81253D77-1075-BCD8-C25B-DE1AED8A63D3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7967160" y="10563311"/>
+              <a:ext cx="341280" cy="341280"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1362,24 +1740,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>306318</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>142349</xdr:rowOff>
+      <xdr:colOff>400182</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>178482</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1050438</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>99804</xdr:rowOff>
+      <xdr:colOff>880422</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>431202</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="44" name="Encre 43">
+            <xdr14:cNvPr id="49" name="Encre 48">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1580458-20D9-40A5-D1E4-AD9EC4ABD207}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75805CF5-3FBC-D1FC-9FF6-EB50D90F4B87}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1387,33 +1765,33 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="11659680" y="10751228"/>
-            <a:ext cx="744120" cy="964697"/>
+            <a:off x="11752200" y="10639271"/>
+            <a:ext cx="480240" cy="252720"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
       <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="44" name="Encre 43">
+            <xdr:cNvPr id="49" name="Encre 48">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1580458-20D9-40A5-D1E4-AD9EC4ABD207}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75805CF5-3FBC-D1FC-9FF6-EB50D90F4B87}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="11624040" y="10715232"/>
-              <a:ext cx="815760" cy="1036329"/>
+              <a:off x="11743200" y="10630271"/>
+              <a:ext cx="497880" cy="270360"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1427,24 +1805,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>445764</xdr:colOff>
+      <xdr:colOff>430284</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>55655</xdr:rowOff>
+      <xdr:rowOff>133067</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1058844</xdr:colOff>
+      <xdr:colOff>913404</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>475055</xdr:rowOff>
+      <xdr:rowOff>445187</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="47" name="Encre 46">
+            <xdr14:cNvPr id="50" name="Encre 49">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1BFA9C8-B5A2-24A2-6DCB-D5EFC3DF9DF2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FD3A746-EFF1-EB94-406E-2A8A85DCFD62}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1452,33 +1830,33 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="10494360" y="12276620"/>
-            <a:ext cx="613080" cy="419400"/>
+            <a:off x="10478880" y="11106313"/>
+            <a:ext cx="483120" cy="312120"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
       <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="47" name="Encre 46">
+            <xdr:cNvPr id="50" name="Encre 49">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1BFA9C8-B5A2-24A2-6DCB-D5EFC3DF9DF2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FD3A746-EFF1-EB94-406E-2A8A85DCFD62}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvPicPr/>
           </xdr:nvPicPr>
           <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
             <a:stretch>
               <a:fillRect/>
             </a:stretch>
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10458360" y="12240620"/>
-              <a:ext cx="684720" cy="491040"/>
+              <a:off x="10469880" y="11097673"/>
+              <a:ext cx="500760" cy="329760"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1492,24 +1870,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>300324</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>467724</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>77627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>947022</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>495420</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>847164</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>412067</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
           <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="62" name="Encre 61">
+            <xdr14:cNvPr id="52" name="Encre 51">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52D85525-299E-9410-3E9E-048A6D42D048}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8559148-52DD-ACED-4312-0F826568E6E0}"/>
                 </a:ext>
               </a:extLst>
             </xdr14:cNvPr>
@@ -1517,18 +1895,83 @@
           </xdr14:nvContentPartPr>
           <xdr14:nvPr macro=""/>
           <xdr14:xfrm>
-            <a:off x="10348920" y="9429239"/>
-            <a:ext cx="1950120" cy="495420"/>
+            <a:off x="10516320" y="11050873"/>
+            <a:ext cx="379440" cy="334440"/>
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
       <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
-            <xdr:cNvPr id="62" name="Encre 61">
+            <xdr:cNvPr id="52" name="Encre 51">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52D85525-299E-9410-3E9E-048A6D42D048}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8559148-52DD-ACED-4312-0F826568E6E0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10507680" y="11041873"/>
+              <a:ext cx="397080" cy="352080"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>656862</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>156014</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>980862</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>377414</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="55" name="Encre 54">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{536F9B52-94ED-F660-3991-EAFD581D5F47}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="12008880" y="13925488"/>
+            <a:ext cx="324000" cy="221400"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="55" name="Encre 54">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{536F9B52-94ED-F660-3991-EAFD581D5F47}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1542,203 +1985,8 @@
           </xdr:blipFill>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10313280" y="9393122"/>
-              <a:ext cx="2021760" cy="568018"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>133700</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>144314</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>902660</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>13458</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
-      <mc:Choice Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId37">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="65" name="Encre 64">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6351C7D6-0EC7-2B1D-F853-2F22C90946EA}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="14092560" y="9580191"/>
-            <a:ext cx="768960" cy="381600"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="65" name="Encre 64">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6351C7D6-0EC7-2B1D-F853-2F22C90946EA}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="14056560" y="9544551"/>
-              <a:ext cx="840600" cy="453240"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>55662</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>167125</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>657222</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>33389</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId39">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="3" name="Encre 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1E76CC0-D6EC-93B1-0C09-8EBB4C448D0B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="11407680" y="13936599"/>
-            <a:ext cx="601560" cy="378720"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="3" name="Encre 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1E76CC0-D6EC-93B1-0C09-8EBB4C448D0B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="11371680" y="13900959"/>
-              <a:ext cx="673200" cy="450360"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:pic>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>166902</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>144445</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1060422</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>269</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
-        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId41">
-          <xdr14:nvContentPartPr>
-            <xdr14:cNvPr id="4" name="Encre 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{254FE118-3574-B911-4CA0-357C1B0D95BB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr14:cNvPr>
-            <xdr14:cNvContentPartPr/>
-          </xdr14:nvContentPartPr>
-          <xdr14:nvPr macro=""/>
-          <xdr14:xfrm>
-            <a:off x="11518920" y="13913919"/>
-            <a:ext cx="893520" cy="368280"/>
-          </xdr14:xfrm>
-        </xdr:contentPart>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:pic>
-          <xdr:nvPicPr>
-            <xdr:cNvPr id="4" name="Encre 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{254FE118-3574-B911-4CA0-357C1B0D95BB}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvPicPr/>
-          </xdr:nvPicPr>
-          <xdr:blipFill>
-            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
-            <a:stretch>
-              <a:fillRect/>
-            </a:stretch>
-          </xdr:blipFill>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="11482920" y="13878279"/>
-              <a:ext cx="965160" cy="439920"/>
+              <a:off x="11999870" y="13916488"/>
+              <a:ext cx="341660" cy="239040"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -1795,15 +2043,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-29T08:31:55.986"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:06:48.688"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1702 372 24575,'-25'1'0,"1"2"0,-1 1 0,0 0 0,-31 11 0,19-5 0,-482 164 0,432-141 0,-262 108 0,17 31 0,278-141 0,-27 18 0,71-41-1365</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1468.72">0 0 24575,'109'117'0,"-6"5"0,88 136 0,-29-28 0,-131-191 0,-18-24 0,-1 0 0,-1 0 0,-1 1 0,0 0 0,-1 1 0,10 25 0,-17-36 0,0 1 0,0-1 0,1 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,1-1 0,0 0 0,-1 0 0,2 0 0,7 5 0,-1-2 0,-1 0 0,0 1 0,0 0 0,-1 1 0,0 0 0,-1 1 0,10 15 0,-16-23 7,1 5-144,1 0 0,0-1-1,1 1 1,-1-1 0,1-1 0,1 1 0,-1-1-1,1 0 1,13 8 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0 24575,'98'50'0,"97"51"0,-174-89 0,-2 0 0,0 2 0,0 0 0,-1 1 0,-1 0 0,0 2 0,19 24 0,66 72 0,-18-22 0,-72-78 0,1-1 0,0 0 0,1-1 0,0-1 0,0 0 0,17 7 0,8 7 0,33 23-1365,-57-36-5461</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1823,17 +2070,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-29T08:35:08.820"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:06:51.272"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1889 390 24575,'-11'1'0,"1"0"0,0 1 0,0 0 0,0 0 0,-13 6 0,-8 2 0,-120 31 0,3 6 0,-185 87 0,228-75 0,18-10 0,-7-13 0,-82 53 0,-68 31 0,202-101 0,-1-3 0,-1-1 0,-91 17 0,126-31 0,0 0 0,0 1 0,0 0 0,0 1 0,0 0 0,1 0 0,-13 7 0,13 2-1365</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1973.36">1 2 24575,'0'4'0,"1"0"0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,5 6 0,20 31 0,-23-36 0,12 13 0,0 1 0,2-2 0,24 21 0,-23-22 0,-1 0 0,-1 1 0,25 33 0,-29-35 0,0-1 0,1 0 0,0 0 0,1-1 0,23 17 0,-2-3 0,-26-18 0,0 0 0,-1 1 0,0 0 0,12 20 0,-14-20 0,1 0 0,0 0 0,1-1 0,0 0 0,15 13 0,7 1 0,-18-15 0,-1 0 0,-1 0 0,1 1 0,11 15 0,-9-9 0,-5-4 0,0 0 0,1 0 0,1-1 0,0-1 0,0 0 0,1 0 0,0-1 0,18 11 0,-18-12 0,0 0 0,-1 0 0,0 1 0,0 1 0,0 0 0,-1 0 0,-1 0 0,8 12 0,-2-4 0,28 27 0,-10-19 0,-21-17 0,-1-1 0,-1 2 0,0-1 0,0 1 0,0 0 0,-1 1 0,11 17 0,-11-15 0,0 0 0,1-1 0,1 0 0,0 0 0,0-1 0,14 10 0,-12-9 0,1 1 0,-1-1 0,-1 2 0,10 13 0,-12-12 0,0 0 0,1 0 0,0-1 0,1-1 0,1 0 0,0 0 0,26 19 0,-24-22-227,-1 1-1,-1 1 1,1 0-1,-2 1 1,11 13-1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16429.34">5417 1 24575,'-26'1'0,"0"1"0,0 1 0,0 1 0,-26 9 0,-97 37 0,114-37 0,-582 183 0,339-94 0,248-90 0,20-9 0,0 1 0,0 0 0,1 0 0,-11 7 0,-1 2 0,-32 14 0,33-17 0,0 0 0,-22 16 0,-82 51 0,13-9 0,-154 108 0,244-161-1365</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="17510.95">3468 112 24575,'37'19'0,"81"46"0,140 95 0,44 27 0,-240-140 0,-45-33 0,0-1 0,1 0 0,20 9 0,-4-4 0,0 1 0,-1 2 0,44 36 0,33 23 0,-40-31 0,-53-35 108,0 1 0,24 29 0,-30-31-350,-1-1 1,2-1 0,0 0 0,0 0-1,1-1 1,20 12 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">773 0 24097,'-773'495'0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1853,15 +2097,15 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-29T08:37:33.574"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:06:59.489"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2135 94 24575,'-5'0'0,"1"0"0,-1 0 0,0 1 0,0 0 0,0 0 0,-6 2 0,-11 3 0,-615 182-108,617-181 84,-458 158-298,-47 14 176,310-118 646,185-56-355,-15 5-1555</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1575.59">0 1 24575,'18'1'0,"0"0"0,0 1 0,-1 2 0,1-1 0,30 13 0,82 40 0,-122-51 0,252 141 0,42 19 0,-202-118 0,144 89 0,-171-88 0,161 99 0,-165-107 0,107 43 0,-36-32 0,-133-46 0,0-1 0,1 1 0,-2 0 0,1 1 0,0 0 0,9 11 0,12 10 0,12 6-1365</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1290 0 24575,'-27'11'0,"-34"19"0,-44 20 0,-42 18 0,-10 7 0,4 2-1061,9-7 1061,17-16 0,31-11 260,26-8-260,20-10 0,13-9 0,7-7 0,10 0 0,2-2 801,-1-2-801,3 4 0,4 0-8191</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1233.49">83 32 24575,'33'13'0,"0"1"0,-1 1 0,-1 2 0,44 31 0,105 95 0,-127-98 0,173 154 0,-163-152 307,-46-35-725,0 0 0,-1 1 0,23 24 0,-28-24-6408</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1881,14 +2125,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-30T09:59:26.032"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:07:17.204"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1670 1 22785,'-1670'1050'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1354 0 24575,'-52'3'0,"-100"17"0,135-17 0,-85 19 0,-147 52 0,170-47 0,-14 9 0,21-6 0,-77 40 0,46-19 0,-16-9 333,77-28-1182,-58 26 0,75-26-5977</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1908,14 +2152,124 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-30T09:59:27.684"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:07:18.641"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 24575,'19'1'0,"-1"1"0,1 1 0,-1 0 0,1 2 0,-1 0 0,26 11 0,-5-2 0,108 35 0,190 38 0,-324-85 0,0 0 0,0 1 0,-1 1 0,1 0 0,-1 0 0,0 2 0,0-1 0,0 1 0,17 13 0,-7-2 0,1 0 0,1-2 0,37 18 0,82 28 0,-98-43 0,62 26 0,119 68 0,-183-90 0,77 29 0,-71-32 0,52 29 0,102 58 0,231 84 0,-430-188 17,11 4-708,27 14 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 24159,'898'898'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink15.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:07:22.391"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1333 0 24575,'-9'1'0,"1"1"0,0-1 0,0 1 0,0 1 0,0 0 0,0 0 0,0 1 0,1-1 0,-11 9 0,-10 3 0,-322 145 0,123-52 0,-71 29 0,-17-20-1365,290-109-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1449.1">157 216 24575,'5'0'0,"-1"1"0,1 0 0,-1 0 0,0 0 0,1 1 0,-1 0 0,0-1 0,0 1 0,0 1 0,6 3 0,6 4 0,66 35 0,-2 4 0,-2 4 0,95 83 0,-130-96 0,-18-16 0,44 33 0,-12-16-1365,-41-31-5461</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink16.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:07:51.362"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1342 1 24575,'-10'9'0,"0"0"0,-1-1 0,0 0 0,0-1 0,-13 7 0,-9 5 0,-274 186 0,185-123 0,-363 229 0,397-259 0,-59 39 0,86-51-1365,39-29-5461</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink17.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:07:53.608"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0 24282,'1052'928'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink18.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:08:07.087"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">899 0 24575,'-18'2'0,"0"0"0,0 2 0,1 0 0,-1 0 0,1 2 0,0 0 0,0 1 0,-16 10 0,-14 11 0,36-19 0,-2-2 0,1 0 0,-21 9 0,19-10 0,1 0 0,0 0 0,1 2 0,-1-1 0,-15 14 0,-53 54 0,32-28 0,13-16 0,-1-2 0,-1-1 0,-46 24 0,74-46 35,-82 51-1435,78-47-5426</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1588.17">0 155 24575,'242'120'0,"-222"-107"0,0 1 0,0 0 0,-2 1 0,0 1 0,29 33 0,-39-41 0,0-1 0,1 0 0,0 0 0,12 6 0,22 16 0,25 24 0,-39-32 0,35 33 0,-63-53 1,-1-1-48,1 0 0,-1 1 0,1-1 0,0 1-1,-1-1 1,1 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0-1 0,0 2 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1962,14 +2316,16 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-29T07:30:01.219"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:05:37.265"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1817 0 24575,'-9'1'0,"0"0"0,0 1 0,0 0 0,1 0 0,-1 1 0,1 0 0,-1 1 0,1 0 0,-8 5 0,-7 2 0,-537 247 0,72-63 0,319-127 0,4-1 0,132-54 0,-60 32 0,-5 2 0,82-41 0,-34 14 0,49-19 0,-1 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,-1 0 0,1-1 0,1 1 0,-1 0 0,0 0 0,-1 4 0,6 7-1365</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">883 32 24575,'0'0'-8191</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="875.63">883 32 24575,'-8'8'0,"-1"-1"0,0-1 0,0 1 0,0-2 0,-16 8 0,-3 2 0,-76 43 0,-96 59 0,126-67 0,-189 132 0,244-170-9,-1 0 0,-35 15 0,25-13-1329,10-4-5488</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2192.37">48 1 24575,'39'35'0,"-25"-24"0,0 2 0,15 18 0,16 23 0,1 1 0,58 89 0,-85-115 0,1-2 0,1 0 0,2-1 0,30 26 0,35 43-1365,-70-75-5461</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -1989,14 +2345,15 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-29T07:30:02.438"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:05:41.076"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0 20859,'2342'701'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">867 155 24575,'-6'0'0,"-1"0"0,1 1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1 1 0,-9 4 0,-43 29 0,46-29 0,-43 32 0,-204 125 0,141-94 0,42-23 0,29-26 0,36-17 0,0 0 0,-17 11 0,18-9-273,-1 0 0,0 0 0,0-1 0,-16 5 0,5-4-6553</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1293.32">1 0 24575,'0'3'0,"1"0"0,0 0 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,4 3 0,3 4 0,132 127 0,-80-79 0,60 71 0,-75-75 0,52 48 0,-35-32 0,-32-32 0,61 67-1365,-80-88-5461</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2016,15 +2373,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-29T07:30:37.508"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:05:44.108"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1673 214 24575,'-16'2'0,"-1"-1"0,0 2 0,1 0 0,0 1 0,-18 8 0,9-5 0,-292 114 0,120-42 0,50-24 0,-439 151 0,470-177 211,59-16-1787</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1693.23">1 1 24575,'138'65'0,"-29"-11"0,-72-39 0,-1 3 0,0 1 0,-2 1 0,57 45 0,-69-47 0,25 15 0,-30-22 0,-1 0 0,-1 1 0,0 1 0,18 19 0,-29-27 0,11 13 0,1 0 0,0-1 0,1 0 0,1-2 0,21 15 0,-30-23 0,0 0 0,-1 0 0,0 1 0,14 18 0,12 10 0,-5-12 0,2-2 0,0 0 0,1-3 0,46 22 0,34 22 0,-69-38 0,79 36 0,-73-39-1365</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1101 1 24575,'-2'0'0,"0"0"0,0 0 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-3 2 0,-9 5 0,-349 174 0,21-12 0,284-140 0,-116 44 0,168-73 6,-13 4-280,1 1 0,0 1 0,0 1-1,-19 11 1,18-6-6552</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2044,15 +2400,14 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-29T07:32:56.764"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:05:51.333"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2001 1 24575,'-21'12'0,"-1"0"0,-1-2 0,0 0 0,0-2 0,-44 10 0,36-9 0,-439 109 0,434-111 0,-66 7 0,65-10 0,-62 14 0,-89 40 0,46-13 0,91-30 0,-1-2 0,0-2 0,-1-3 0,0-2 0,-54-1 0,98-6 0,0 1 0,0 1 0,0 0 0,-13 3 0,19-3 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 1 0,1 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 1 0,0-1 0,-3 4 0,-2 4 36,-1-1 0,-1 0 0,0-1 0,0 0 0,0 0 0,-12 7-1,-66 34-77,1 0-1532</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1799.64">117 1 24575,'20'5'0,"44"23"0,46 21 0,42 24 0,30 15 0,10 2-983,-11-3 0,-22-11 512,-17-9 471,-27-16 778,-29-16-778,-22-14 402,-24-5-402</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 24575,'33'29'0,"-26"-24"0,1 1 0,-2 1 0,1-1 0,10 13 0,-4-3 0,1 0 0,1-1 0,0-1 0,1-1 0,1 0 0,18 10 0,-10-6 0,44 39 0,-38-25 0,1-3 0,1 0 0,2-2 0,44 25 0,84 52 0,-142-90-1365,0-2-5461</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2072,15 +2427,15 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-29T07:39:28.213"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:06:03.079"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2161 0 24575,'-29'1'0,"-1"2"0,1 0 0,-43 12 0,-85 32 0,127-37 0,-671 226 0,261-87 0,-135 66 0,493-181-1365</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1560.23">0 335 24575,'10'0'0,"-1"1"0,0 0 0,0 1 0,-1 0 0,1 0 0,0 1 0,10 5 0,58 32 0,-21-9 0,48 18 0,250 129 0,-53-16-1365</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">899 1 24575,'-2'2'0,"-1"0"0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 0,-5 1 0,-11 7 0,-135 96 0,37-24 0,85-61 0,-194 121 0,191-121 0,-45 35 0,56-38 0,0-1 0,-1-1 0,0-1 0,-36 15 0,32-18-1365,7-1-5461</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1212.23">1 155 24575,'4'1'0,"-1"0"0,1 0 0,0 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,4 5 0,4 2 0,248 170 0,-12 21 0,-183-144 253,-36-32-792,0 1-1,36 42 1,-54-53-6287</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2100,15 +2455,15 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-29T07:40:20.528"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:06:05.696"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1636 0 24575,'-19'18'0,"-1"-2"0,-1 0 0,-31 18 0,31-21 0,-478 303 0,384-247 0,-189 83 0,167-78 0,-176 88 0,179-90-1365</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1606.66">24 183 24575,'11'9'0,"0"0"0,0-1 0,1-1 0,13 8 0,16 9 0,128 81 0,298 137 0,-448-234 0,1 0 0,0-1 0,29 7 0,-41-12 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 1 0,11 9 0,19 9 0,22 7 0,-25-11 0,2-2 0,45 15 0,-55-22-1365</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">784 33 24575,'-5'0'0,"-18"10"0,-25 20 0,-16 9 0,-13 4 0,-3 0 0,6-3 0,6-7 0,8-11 0,10-2 0,8-5 0,6 0 0,3-3 0,3 3 0,1-3 0,5 4 0,1-2 0,6-4-8191</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1414.34">10 1 24575,'240'230'0,"-53"-48"0,-160-149 0,3 2 0,-21-26-341,0 0 0,0 0-1,12 18 1,-8-7-6485</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2128,17 +2483,15 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-11-29T07:34:47.889"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-12-14T20:06:13.869"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.2" units="cm"/>
-      <inkml:brushProperty name="height" value="0.2" units="cm"/>
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">2008 243 24575,'-66'20'0,"-89"39"0,111-41 0,-368 177 0,236-107 0,-109 60 0,216-110 0,-93 57 0,6-1 0,123-80 0,27-13 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 1 0,-7 6 0,12-2-1365</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1255.82">395 0 24575,'7'1'0,"0"0"0,-1 0 0,1 1 0,-1-1 0,0 1 0,1 1 0,-1-1 0,7 5 0,10 4 0,755 342 0,-583-260 0,-154-71 0,53 37 0,31 18 0,-25-30 0,74 40 0,-159-77-46,0 1 0,17 15-1,-17-13-1179</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-57310.07">1704 1551 24575,'-24'8'0,"0"1"0,1 1 0,0 1 0,-41 26 0,18-9 0,-36 17 0,-2-3 0,-117 40 0,41-15 0,134-56 0,-93 39 0,-143 37 0,240-81 0,1 2 0,-30 13 0,44-17 0,0-1 0,1 1 0,0 1 0,0-1 0,0 1 0,1 0 0,-1 1 0,1-1 0,0 1 0,1 0 0,-6 8 0,0 2 41,-2-1-1,0 0 1,-1-1 0,0 0-1,-27 20 1,-20 22-1650</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="-55779.75">1 1460 24575,'94'61'0,"-36"-25"0,400 265 0,-444-291 0,1-1 0,0-1 0,0-1 0,0 0 0,1-1 0,0 0 0,1-2 0,18 4 0,-24-6 0,0 1 0,0 0 0,0 1 0,0 0 0,0 0 0,16 10 0,53 43 0,-55-38 0,37 22 0,-17-16 0,-1 1 0,-1 3 0,42 37 0,56 40 0,-59-47 0,43 23 0,-83-55 0,-28-19 0,-1 1 0,1 0 0,-1 1 0,-1 0 0,0 1 0,-1 0 0,15 18 0,-18-19-94,1 0-1,0 0 1,0-1-1,1 0 1,0-1 0,1 0-1,18 10 1,-20-11-516</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1014 61 24575,'-21'6'0,"-29"11"0,-31 20 0,-23 13 0,-21 9 0,1 0 0,6-5 0,17-1 0,16-10 0,16-7 0,16-9 0,16-4 0,9-6 0,10-6-8191</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1286.05">115 0 24575,'3'1'0,"0"0"0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 1 0,1 0 0,2 4 0,4 3 0,69 45 0,9 8 0,20 40 0,-83-80 0,-2 0 0,31 41 0,-33-38 0,1 0 0,33 29 0,-40-42-227,-1 2-1,-1-1 1,0 2-1,0 0 1,17 31-1,-19-27-6598</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -2434,8 +2787,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="57" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" zoomScale="57" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2475,14 +2828,14 @@
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="31"/>
       <c r="F3" s="35" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="G3" s="30"/>
       <c r="H3" s="36"/>
@@ -2492,25 +2845,25 @@
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
       <c r="E4" s="34"/>
       <c r="F4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="19" t="s">
         <v>6</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
@@ -2522,50 +2875,50 @@
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="38"/>
       <c r="B7" s="46"/>
       <c r="C7" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="E7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="F7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="G7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="H7" s="21" t="s">
         <v>20</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>21</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
@@ -2649,12 +3002,8 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="A9" s="22"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
       <c r="E9" s="14"/>
@@ -2699,10 +3048,10 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
@@ -2748,10 +3097,10 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -2797,10 +3146,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -2815,7 +3164,7 @@
       <c r="M12"/>
       <c r="N12"/>
       <c r="O12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P12"/>
       <c r="Q12"/>
@@ -2848,10 +3197,10 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -2897,10 +3246,10 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
@@ -3126,7 +3475,7 @@
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="43"/>
       <c r="C19" s="43"/>
@@ -3173,10 +3522,10 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
@@ -3491,7 +3840,7 @@
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="43"/>
       <c r="C27" s="43"/>
@@ -3537,12 +3886,8 @@
       <c r="AQ27"/>
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>39</v>
-      </c>
+      <c r="A28" s="27"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
@@ -4203,11 +4548,11 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d67bd3f6-a29a-4795-b867-0d25e089f636"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d67bd3f6-a29a-4795-b867-0d25e089f636"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="5c6232be-ce18-4d83-a1a2-d9e20b7892ec"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>

</xml_diff>